<commit_message>
Update summary and Excel file from workflow run
</commit_message>
<xml_diff>
--- a/certificati_iso_date_with_status.xlsx
+++ b/certificati_iso_date_with_status.xlsx
@@ -646,7 +646,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>❌ EXPIRED 3750 days ago</t>
+          <t>❌ EXPIRED 3753 days ago</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>⚠️ Expires in 29 days</t>
+          <t>⚠️ Expires in 26 days</t>
         </is>
       </c>
     </row>
@@ -692,7 +692,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>⚠️ Expires in 29 days</t>
+          <t>⚠️ Expires in 26 days</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>⚠️ Expires in 29 days</t>
+          <t>⚠️ Expires in 26 days</t>
         </is>
       </c>
     </row>

</xml_diff>